<commit_message>
write to sub files
</commit_message>
<xml_diff>
--- a/files/sub/sub1.xlsx
+++ b/files/sub/sub1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
   <workbookPr showInkAnnotation="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nhancao/Desktop/"/>
     </mc:Choice>
@@ -23,9 +23,18 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>nhancv</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -342,8 +351,8 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1">
-        <v>1</v>
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>